<commit_message>
description for pipeline behaviour
</commit_message>
<xml_diff>
--- a/doc/dependencies_pipeline.xlsx
+++ b/doc/dependencies_pipeline.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="pipeline behaviour" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>lw v1, 0(v1)</t>
   </si>
@@ -43,6 +43,39 @@
   </si>
   <si>
     <t>Assuming a 5-stage pipeline</t>
+  </si>
+  <si>
+    <t>lw r6, 0(r6)</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Reg</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>Pipeline Stage</t>
+  </si>
+  <si>
+    <t>Functional Unit</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>reg[r6]</t>
+  </si>
+  <si>
+    <t>addr = 0 + reg[r6]</t>
+  </si>
+  <si>
+    <t>mem[addr]</t>
+  </si>
+  <si>
+    <t>reg[r6] = mem[addr]</t>
   </si>
 </sst>
 </file>
@@ -102,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -138,11 +171,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -181,6 +232,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -613,12 +672,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="6" width="14.7109375" style="1" customWidth="1"/>
+    <col min="7" max="44" width="4.7109375" style="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added diagram for 6 and 7 stages
</commit_message>
<xml_diff>
--- a/doc/dependencies_pipeline.xlsx
+++ b/doc/dependencies_pipeline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="25">
   <si>
     <t>lw v1, 0(v1)</t>
   </si>
@@ -76,6 +76,21 @@
   </si>
   <si>
     <t>reg[r6] = mem[addr]</t>
+  </si>
+  <si>
+    <t>6-stage pipeline</t>
+  </si>
+  <si>
+    <t>IF1</t>
+  </si>
+  <si>
+    <t>IF2</t>
+  </si>
+  <si>
+    <t>IF3</t>
+  </si>
+  <si>
+    <t>7-stage</t>
   </si>
 </sst>
 </file>
@@ -193,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -240,6 +255,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -553,12 +569,12 @@
     <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -599,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -621,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -644,7 +660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -661,6 +677,342 @@
         <v>4</v>
       </c>
       <c r="J7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -674,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>